<commit_message>
main alter rating not working still
</commit_message>
<xml_diff>
--- a/top100BooksByMedium.xlsx
+++ b/top100BooksByMedium.xlsx
@@ -391,6 +391,13 @@
           <t>F. Scott Fitzgerald</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.91
+</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -408,6 +415,13 @@
           <t>Joseph Heller</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.98
+</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -425,6 +439,11 @@
           <t>Jack Kerouac</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -442,6 +461,13 @@
           <t xml:space="preserve">Harper Lee </t>
         </is>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.27
+</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -457,6 +483,13 @@
       <c r="C6" t="inlineStr">
         <is>
           <t>J. R. R. Tolkien</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.50
+</t>
         </is>
       </c>
     </row>

</xml_diff>